<commit_message>
Finished updating some files.
</commit_message>
<xml_diff>
--- a/Basic_File.xlsx
+++ b/Basic_File.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27030"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1991FF59-BE85-4078-ACCF-6A593CED2613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FB752D3-AF82-483C-A358-B6A3E53C7F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>D</t>
   </si>
   <si>
-    <t>jO3</t>
+    <t>jO1D</t>
   </si>
   <si>
     <t>2OH</t>
@@ -490,9 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>